<commit_message>
Adjusted mistake across all notebook and dashboards
</commit_message>
<xml_diff>
--- a/data/processed/feature_importance.xlsx
+++ b/data/processed/feature_importance.xlsx
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1498</v>
+        <v>1333</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>792</v>
+        <v>781</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>726</v>
+        <v>736</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>661</v>
+        <v>606</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>580</v>
+        <v>558</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
@@ -531,11 +531,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>AMT_ANNUITY</t>
+          <t>YEARS_EMPLOYED</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>523</v>
+        <v>478</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
@@ -548,7 +548,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>497</v>
+        <v>457</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
@@ -557,11 +557,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>YEARS_EMPLOYED</t>
+          <t>YEARS_REGISTRATION</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>483</v>
+        <v>454</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
@@ -570,11 +570,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>YEARS_REGISTRATION</t>
+          <t>AMT_ANNUITY</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>449</v>
+        <v>427</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
@@ -587,7 +587,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
@@ -613,7 +613,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
@@ -665,7 +665,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
@@ -691,7 +691,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
@@ -704,7 +704,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
@@ -713,11 +713,11 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>NAME_EDUCATION_TYPE</t>
+          <t>prev_cnt_revolving_refused</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C22" t="n">
         <v>21</v>
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C23" t="n">
         <v>22</v>
@@ -739,11 +739,11 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>prev_cnt_revolving_refused</t>
+          <t>NAME_EDUCATION_TYPE</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C24" t="n">
         <v>23</v>
@@ -752,11 +752,11 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>NAME_HOUSING_TYPE</t>
+          <t>FLAG_WORK_PHONE</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C25" t="n">
         <v>24</v>
@@ -765,11 +765,11 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>FLAG_DOCUMENT_3</t>
+          <t>NAME_CONTRACT_TYPE</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C26" t="n">
         <v>25</v>
@@ -778,11 +778,11 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>FLAG_WORK_PHONE</t>
+          <t>NAME_HOUSING_TYPE</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C27" t="n">
         <v>26</v>
@@ -791,11 +791,11 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>NAME_CONTRACT_TYPE</t>
+          <t>FLAG_DOCUMENT_3</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C28" t="n">
         <v>27</v>
@@ -804,11 +804,11 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>bur_has_history</t>
+          <t>REG_CITY_NOT_LIVE_CITY</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C29" t="n">
         <v>28</v>
@@ -817,11 +817,11 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>prev_cnt_revolving_canceled</t>
+          <t>bur_has_history</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C30" t="n">
         <v>29</v>
@@ -830,11 +830,11 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>REG_CITY_NOT_LIVE_CITY</t>
+          <t>prev_cnt_revolving_canceled</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C31" t="n">
         <v>30</v>
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C32" t="n">
         <v>31</v>
@@ -856,11 +856,11 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>NAME_INCOME_TYPE</t>
+          <t>FLAG_PHONE</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C33" t="n">
         <v>32</v>
@@ -869,11 +869,11 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>FLAG_PHONE</t>
+          <t>NAME_INCOME_TYPE</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C34" t="n">
         <v>33</v>
@@ -886,7 +886,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C35" t="n">
         <v>34</v>
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37" t="n">
         <v>36</v>

</xml_diff>